<commit_message>
reorganize the code. SMMEst.py saves all class and DoSMMEst does the estimation and plot. no more differences DENI with 1 or 2 signals. always 2 now.
</commit_message>
<xml_diff>
--- a/workingfolder/OtherData/CPICQ.xlsx
+++ b/workingfolder/OtherData/CPICQ.xlsx
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:B111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,7 +402,7 @@
         <v>34700</v>
       </c>
       <c r="B2">
-        <v>2.962008953094482</v>
+        <v>2.962002992630005</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -410,7 +410,7 @@
         <v>34790</v>
       </c>
       <c r="B3">
-        <v>3.005115032196045</v>
+        <v>3.005122900009155</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -418,7 +418,7 @@
         <v>34881</v>
       </c>
       <c r="B4">
-        <v>2.984127044677734</v>
+        <v>2.984125137329102</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -426,7 +426,7 @@
         <v>34973</v>
       </c>
       <c r="B5">
-        <v>3.032217264175415</v>
+        <v>3.032219171524048</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -434,7 +434,7 @@
         <v>35065</v>
       </c>
       <c r="B6">
-        <v>2.814258813858032</v>
+        <v>2.814259052276611</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -442,7 +442,7 @@
         <v>35156</v>
       </c>
       <c r="B7">
-        <v>2.66914963722229</v>
+        <v>2.669142007827759</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -450,7 +450,7 @@
         <v>35247</v>
       </c>
       <c r="B8">
-        <v>2.651048183441162</v>
+        <v>2.651050090789795</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -458,7 +458,7 @@
         <v>35339</v>
       </c>
       <c r="B9">
-        <v>2.636419296264648</v>
+        <v>2.636411905288696</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -466,7 +466,7 @@
         <v>35431</v>
       </c>
       <c r="B10">
-        <v>2.433089971542358</v>
+        <v>2.433090209960938</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -482,7 +482,7 @@
         <v>35612</v>
       </c>
       <c r="B12">
-        <v>2.222222328186035</v>
+        <v>2.222220420837402</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -490,7 +490,7 @@
         <v>35704</v>
       </c>
       <c r="B13">
-        <v>2.270011901855469</v>
+        <v>2.270013809204102</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -498,7 +498,7 @@
         <v>35796</v>
       </c>
       <c r="B14">
-        <v>2.256531953811646</v>
+        <v>2.256533861160278</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -506,7 +506,7 @@
         <v>35886</v>
       </c>
       <c r="B15">
-        <v>2.243211269378662</v>
+        <v>2.243213176727295</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -522,7 +522,7 @@
         <v>36069</v>
       </c>
       <c r="B17">
-        <v>2.45327091217041</v>
+        <v>2.453269243240356</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -538,7 +538,7 @@
         <v>36251</v>
       </c>
       <c r="B19">
-        <v>1.963048458099365</v>
+        <v>1.963053822517395</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -546,7 +546,7 @@
         <v>36342</v>
       </c>
       <c r="B20">
-        <v>2.066590070724487</v>
+        <v>2.066593647003174</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -554,7 +554,7 @@
         <v>36434</v>
       </c>
       <c r="B21">
-        <v>1.88141393661499</v>
+        <v>1.881415724754333</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -562,7 +562,7 @@
         <v>36526</v>
       </c>
       <c r="B22">
-        <v>2.447353363037109</v>
+        <v>2.447355270385742</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -570,7 +570,7 @@
         <v>36617</v>
       </c>
       <c r="B23">
-        <v>2.548131465911865</v>
+        <v>2.548131227493286</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -586,7 +586,7 @@
         <v>36800</v>
       </c>
       <c r="B25">
-        <v>2.574146509170532</v>
+        <v>2.574150085449219</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -594,7 +594,7 @@
         <v>36892</v>
       </c>
       <c r="B26">
-        <v>2.611111164093018</v>
+        <v>2.611109495162964</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -602,7 +602,7 @@
         <v>36982</v>
       </c>
       <c r="B27">
-        <v>2.705687522888184</v>
+        <v>2.705683946609497</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -610,7 +610,7 @@
         <v>37073</v>
       </c>
       <c r="B28">
-        <v>2.633022546768188</v>
+        <v>2.633024215698242</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -618,7 +618,7 @@
         <v>37165</v>
       </c>
       <c r="B29">
-        <v>2.782324075698853</v>
+        <v>2.782319068908691</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -634,7 +634,7 @@
         <v>37347</v>
       </c>
       <c r="B31">
-        <v>2.25806450843811</v>
+        <v>2.258062839508057</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -642,7 +642,7 @@
         <v>37438</v>
       </c>
       <c r="B32">
-        <v>2.244788885116577</v>
+        <v>2.244787216186523</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -650,7 +650,7 @@
         <v>37530</v>
       </c>
       <c r="B33">
-        <v>1.963906526565552</v>
+        <v>1.963913083076477</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -658,7 +658,7 @@
         <v>37622</v>
       </c>
       <c r="B34">
-        <v>1.744186043739319</v>
+        <v>1.744187712669373</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -666,7 +666,7 @@
         <v>37712</v>
       </c>
       <c r="B35">
-        <v>1.472134590148926</v>
+        <v>1.472136259078979</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -674,7 +674,7 @@
         <v>37803</v>
       </c>
       <c r="B36">
-        <v>1.254573941230774</v>
+        <v>1.254570722579956</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -682,7 +682,7 @@
         <v>37895</v>
       </c>
       <c r="B37">
-        <v>1.093180656433105</v>
+        <v>1.093175888061523</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -698,7 +698,7 @@
         <v>38078</v>
       </c>
       <c r="B39">
-        <v>1.86528491973877</v>
+        <v>1.865288138389587</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -706,7 +706,7 @@
         <v>38169</v>
       </c>
       <c r="B40">
-        <v>1.961796641349792</v>
+        <v>1.961798191070557</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -714,7 +714,7 @@
         <v>38261</v>
       </c>
       <c r="B41">
-        <v>2.265705347061157</v>
+        <v>2.265710115432739</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -722,7 +722,7 @@
         <v>38353</v>
       </c>
       <c r="B42">
-        <v>2.352941274642944</v>
+        <v>2.352944374084473</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -730,7 +730,7 @@
         <v>38443</v>
       </c>
       <c r="B43">
-        <v>2.034588098526001</v>
+        <v>2.034587860107422</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -738,7 +738,7 @@
         <v>38534</v>
       </c>
       <c r="B44">
-        <v>1.924050688743591</v>
+        <v>1.924052119255066</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -746,7 +746,7 @@
         <v>38626</v>
       </c>
       <c r="B45">
-        <v>2.114803552627563</v>
+        <v>2.114802122116089</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -754,7 +754,7 @@
         <v>38718</v>
       </c>
       <c r="B46">
-        <v>2.098950624465942</v>
+        <v>2.098948955535889</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -762,7 +762,7 @@
         <v>38808</v>
       </c>
       <c r="B47">
-        <v>2.6420738697052</v>
+        <v>2.642067670822144</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -770,7 +770,7 @@
         <v>38899</v>
       </c>
       <c r="B48">
-        <v>2.930948734283447</v>
+        <v>2.930945873260498</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -778,7 +778,7 @@
         <v>38991</v>
       </c>
       <c r="B49">
-        <v>2.613412141799927</v>
+        <v>2.61341381072998</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -786,7 +786,7 @@
         <v>39083</v>
       </c>
       <c r="B50">
-        <v>2.505139589309692</v>
+        <v>2.50513768196106</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -794,7 +794,7 @@
         <v>39173</v>
       </c>
       <c r="B51">
-        <v>2.181641578674316</v>
+        <v>2.181643724441528</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -802,7 +802,7 @@
         <v>39264</v>
       </c>
       <c r="B52">
-        <v>2.101351261138916</v>
+        <v>2.101353168487549</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -810,7 +810,7 @@
         <v>39356</v>
       </c>
       <c r="B53">
-        <v>2.435367584228516</v>
+        <v>2.435364246368408</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -818,7 +818,7 @@
         <v>39448</v>
       </c>
       <c r="B54">
-        <v>2.388524293899536</v>
+        <v>2.388523817062378</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -826,7 +826,7 @@
         <v>39539</v>
       </c>
       <c r="B55">
-        <v>2.391726016998291</v>
+        <v>2.391724824905396</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -834,7 +834,7 @@
         <v>39630</v>
       </c>
       <c r="B56">
-        <v>2.438620805740356</v>
+        <v>2.438619136810303</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -842,7 +842,7 @@
         <v>39722</v>
       </c>
       <c r="B57">
-        <v>1.762459635734558</v>
+        <v>1.762461423873901</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -850,7 +850,7 @@
         <v>39814</v>
       </c>
       <c r="B58">
-        <v>1.787613153457642</v>
+        <v>1.787616729736328</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -858,7 +858,7 @@
         <v>39904</v>
       </c>
       <c r="B59">
-        <v>1.711972713470459</v>
+        <v>1.711974382400513</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -866,7 +866,7 @@
         <v>39995</v>
       </c>
       <c r="B60">
-        <v>1.479837417602539</v>
+        <v>1.479837775230408</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -874,7 +874,7 @@
         <v>40087</v>
       </c>
       <c r="B61">
-        <v>1.823671817779541</v>
+        <v>1.823668837547302</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -882,7 +882,7 @@
         <v>40179</v>
       </c>
       <c r="B62">
-        <v>1.159205198287964</v>
+        <v>1.159204602241516</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -890,7 +890,7 @@
         <v>40269</v>
       </c>
       <c r="B63">
-        <v>0.9501990079879761</v>
+        <v>0.9501993060112</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -898,7 +898,7 @@
         <v>40360</v>
       </c>
       <c r="B64">
-        <v>0.8143870234489441</v>
+        <v>0.8143872022628784</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -906,7 +906,7 @@
         <v>40452</v>
       </c>
       <c r="B65">
-        <v>0.6618948578834534</v>
+        <v>0.6618974208831787</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -914,7 +914,7 @@
         <v>40544</v>
       </c>
       <c r="B66">
-        <v>1.209785223007202</v>
+        <v>1.20978057384491</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -922,7 +922,7 @@
         <v>40634</v>
       </c>
       <c r="B67">
-        <v>1.583677649497986</v>
+        <v>1.583680391311646</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -930,7 +930,7 @@
         <v>40725</v>
       </c>
       <c r="B68">
-        <v>1.987722754478455</v>
+        <v>1.987721681594849</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -938,7 +938,7 @@
         <v>40817</v>
       </c>
       <c r="B69">
-        <v>2.276662588119507</v>
+        <v>2.276660919189453</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -946,7 +946,7 @@
         <v>40909</v>
       </c>
       <c r="B70">
-        <v>2.248337507247925</v>
+        <v>2.248338460922241</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -954,7 +954,7 @@
         <v>41000</v>
       </c>
       <c r="B71">
-        <v>2.192285537719727</v>
+        <v>2.192283153533936</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -970,7 +970,7 @@
         <v>41183</v>
       </c>
       <c r="B73">
-        <v>1.899694323539734</v>
+        <v>1.899697661399841</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -978,7 +978,7 @@
         <v>41275</v>
       </c>
       <c r="B74">
-        <v>1.8890221118927</v>
+        <v>1.889026284217834</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -986,7 +986,7 @@
         <v>41365</v>
       </c>
       <c r="B75">
-        <v>1.623095273971558</v>
+        <v>1.62309741973877</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -994,7 +994,7 @@
         <v>41456</v>
       </c>
       <c r="B76">
-        <v>1.751936793327332</v>
+        <v>1.751937031745911</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1002,7 +1002,7 @@
         <v>41548</v>
       </c>
       <c r="B77">
-        <v>1.740856647491455</v>
+        <v>1.740855097770691</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1010,7 +1010,7 @@
         <v>41640</v>
       </c>
       <c r="B78">
-        <v>1.645660996437073</v>
+        <v>1.645658254623413</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1018,7 +1018,7 @@
         <v>41730</v>
       </c>
       <c r="B79">
-        <v>1.922862648963928</v>
+        <v>1.922862410545349</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1026,7 +1026,7 @@
         <v>41821</v>
       </c>
       <c r="B80">
-        <v>1.740945935249329</v>
+        <v>1.740945339202881</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1034,7 +1034,7 @@
         <v>41913</v>
       </c>
       <c r="B81">
-        <v>1.622419476509094</v>
+        <v>1.622418165206909</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1042,7 +1042,7 @@
         <v>42005</v>
       </c>
       <c r="B82">
-        <v>1.745377659797668</v>
+        <v>1.74537980556488</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1050,7 +1050,7 @@
         <v>42095</v>
       </c>
       <c r="B83">
-        <v>1.777267575263977</v>
+        <v>1.777263283729553</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1058,7 +1058,7 @@
         <v>42186</v>
       </c>
       <c r="B84">
-        <v>1.897096157073975</v>
+        <v>1.897095680236816</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1066,7 +1066,7 @@
         <v>42278</v>
       </c>
       <c r="B85">
-        <v>2.071507215499878</v>
+        <v>2.071506261825562</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1074,7 +1074,7 @@
         <v>42370</v>
       </c>
       <c r="B86">
-        <v>2.163610219955444</v>
+        <v>2.142422437667847</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1082,7 +1082,7 @@
         <v>42461</v>
       </c>
       <c r="B87">
-        <v>2.218834638595581</v>
+        <v>2.262210845947266</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1090,7 +1090,7 @@
         <v>42552</v>
       </c>
       <c r="B88">
-        <v>2.216459274291992</v>
+        <v>2.271121025085449</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1098,7 +1098,7 @@
         <v>42644</v>
       </c>
       <c r="B89">
-        <v>2.213071584701538</v>
+        <v>2.197124242782593</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1106,7 +1106,7 @@
         <v>42736</v>
       </c>
       <c r="B90">
-        <v>2.004358291625977</v>
+        <v>2.04584789276123</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1114,7 +1114,7 @@
         <v>42826</v>
       </c>
       <c r="B91">
-        <v>1.729343056678772</v>
+        <v>1.699123024940491</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1122,7 +1122,7 @@
         <v>42917</v>
       </c>
       <c r="B92">
-        <v>1.680276989936829</v>
+        <v>1.595390319824219</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1130,7 +1130,7 @@
         <v>43009</v>
       </c>
       <c r="B93">
-        <v>1.76869010925293</v>
+        <v>1.770164847373962</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1138,7 +1138,7 @@
         <v>43101</v>
       </c>
       <c r="B94">
-        <v>2.065015554428101</v>
+        <v>2.065795660018921</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1146,7 +1146,7 @@
         <v>43191</v>
       </c>
       <c r="B95">
-        <v>2.267652988433838</v>
+        <v>2.265379667282104</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1154,7 +1154,7 @@
         <v>43282</v>
       </c>
       <c r="B96">
-        <v>2.261080026626587</v>
+        <v>2.251874208450317</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1162,7 +1162,119 @@
         <v>43374</v>
       </c>
       <c r="B97">
-        <v>2.203789710998535</v>
+        <v>2.197809457778931</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="2">
+        <v>43466</v>
+      </c>
+      <c r="B98">
+        <v>2.05131721496582</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="2">
+        <v>43556</v>
+      </c>
+      <c r="B99">
+        <v>2.134792566299438</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="2">
+        <v>43647</v>
+      </c>
+      <c r="B100">
+        <v>2.353148937225342</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="2">
+        <v>43739</v>
+      </c>
+      <c r="B101">
+        <v>2.234418869018555</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="2">
+        <v>43831</v>
+      </c>
+      <c r="B102">
+        <v>2.117206573486328</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B103">
+        <v>1.195309042930603</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B104">
+        <v>1.724944114685059</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="2">
+        <v>44105</v>
+      </c>
+      <c r="B105">
+        <v>1.596286773681641</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B106">
+        <v>1.660072803497314</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="2">
+        <v>44287</v>
+      </c>
+      <c r="B107">
+        <v>4.447394847869873</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="2">
+        <v>44378</v>
+      </c>
+      <c r="B108">
+        <v>4.036748886108398</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="2">
+        <v>44470</v>
+      </c>
+      <c r="B109">
+        <v>5.476613521575928</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="2">
+        <v>44562</v>
+      </c>
+      <c r="B110">
+        <v>6.436047077178955</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="2">
+        <v>44652</v>
+      </c>
+      <c r="B111">
+        <v>6.011281490325928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated OtherData in July 2023
</commit_message>
<xml_diff>
--- a/workingfolder/OtherData/CPICQ.xlsx
+++ b/workingfolder/OtherData/CPICQ.xlsx
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B111"/>
+  <dimension ref="A1:B102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1205,78 +1205,6 @@
         <v>2.117206573486328</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
-      <c r="A103" s="2">
-        <v>43922</v>
-      </c>
-      <c r="B103">
-        <v>1.195309042930603</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
-      <c r="A104" s="2">
-        <v>44013</v>
-      </c>
-      <c r="B104">
-        <v>1.724944114685059</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="A105" s="2">
-        <v>44105</v>
-      </c>
-      <c r="B105">
-        <v>1.596286773681641</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106" s="2">
-        <v>44197</v>
-      </c>
-      <c r="B106">
-        <v>1.660072803497314</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="A107" s="2">
-        <v>44287</v>
-      </c>
-      <c r="B107">
-        <v>4.447394847869873</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="2">
-        <v>44378</v>
-      </c>
-      <c r="B108">
-        <v>4.036748886108398</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" s="2">
-        <v>44470</v>
-      </c>
-      <c r="B109">
-        <v>5.476613521575928</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110" s="2">
-        <v>44562</v>
-      </c>
-      <c r="B110">
-        <v>6.436047077178955</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111" s="2">
-        <v>44652</v>
-      </c>
-      <c r="B111">
-        <v>6.011281490325928</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated UCSV estiamtes and related data
</commit_message>
<xml_diff>
--- a/workingfolder/OtherData/CPICQ.xlsx
+++ b/workingfolder/OtherData/CPICQ.xlsx
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B102"/>
+  <dimension ref="A1:B114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1138,7 +1138,7 @@
         <v>43101</v>
       </c>
       <c r="B94">
-        <v>2.065795660018921</v>
+        <v>2.122782707214355</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1146,7 +1146,7 @@
         <v>43191</v>
       </c>
       <c r="B95">
-        <v>2.265379667282104</v>
+        <v>2.245511293411255</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1154,7 +1154,7 @@
         <v>43282</v>
       </c>
       <c r="B96">
-        <v>2.251874208450317</v>
+        <v>2.197686433792114</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1162,7 +1162,7 @@
         <v>43374</v>
       </c>
       <c r="B97">
-        <v>2.197809457778931</v>
+        <v>2.24852728843689</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1170,7 +1170,7 @@
         <v>43466</v>
       </c>
       <c r="B98">
-        <v>2.05131721496582</v>
+        <v>2.054852485656738</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1178,7 +1178,7 @@
         <v>43556</v>
       </c>
       <c r="B99">
-        <v>2.134792566299438</v>
+        <v>2.121228933334351</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1186,7 +1186,7 @@
         <v>43647</v>
       </c>
       <c r="B100">
-        <v>2.353148937225342</v>
+        <v>2.344321250915527</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1194,7 +1194,7 @@
         <v>43739</v>
       </c>
       <c r="B101">
-        <v>2.234418869018555</v>
+        <v>2.253693580627441</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1202,7 +1202,103 @@
         <v>43831</v>
       </c>
       <c r="B102">
-        <v>2.117206573486328</v>
+        <v>2.123221397399902</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B103">
+        <v>1.176671504974365</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B104">
+        <v>1.706722378730774</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="2">
+        <v>44105</v>
+      </c>
+      <c r="B105">
+        <v>1.633168458938599</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B106">
+        <v>1.660865187644958</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="2">
+        <v>44287</v>
+      </c>
+      <c r="B107">
+        <v>4.408313751220703</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="2">
+        <v>44378</v>
+      </c>
+      <c r="B108">
+        <v>4.022122859954834</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="2">
+        <v>44470</v>
+      </c>
+      <c r="B109">
+        <v>5.522685050964355</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="2">
+        <v>44562</v>
+      </c>
+      <c r="B110">
+        <v>6.452416896820068</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="2">
+        <v>44652</v>
+      </c>
+      <c r="B111">
+        <v>5.884917736053467</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="2">
+        <v>44743</v>
+      </c>
+      <c r="B112">
+        <v>6.64294958114624</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="2">
+        <v>44835</v>
+      </c>
+      <c r="B113">
+        <v>5.703855991363525</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B114">
+        <v>5.602568626403809</v>
       </c>
     </row>
   </sheetData>

</xml_diff>